<commit_message>
mise à jour du tableau comparatif
</commit_message>
<xml_diff>
--- a/etude-comparative/comparatif.xlsx
+++ b/etude-comparative/comparatif.xlsx
@@ -111,9 +111,6 @@
     <t xml:space="preserve">Importation massive </t>
   </si>
   <si>
-    <t>Monitoring distribué (asservissement)</t>
-  </si>
-  <si>
     <t>Gestion des escalades</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>Mise à jour en masse</t>
+  </si>
+  <si>
+    <t>Monitoring distribué (aggrégation)</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J3:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +702,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6">
@@ -785,25 +785,37 @@
         <v>1</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3</v>
+      </c>
       <c r="H7" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="5" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="6">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>3</v>
+      </c>
       <c r="H8" s="6">
         <v>2</v>
       </c>
@@ -811,7 +823,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6">
@@ -833,13 +845,19 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
       <c r="H10" s="6">
         <v>2</v>
       </c>
@@ -847,15 +865,21 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
       <c r="H11" s="6">
         <v>1</v>
       </c>
@@ -913,9 +937,15 @@
       <c r="D14" s="6">
         <v>1</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
       <c r="H14" s="6">
         <v>1</v>
       </c>
@@ -929,9 +959,15 @@
         <v>1</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="E15" s="6">
+        <v>3</v>
+      </c>
+      <c r="F15" s="6">
+        <v>2</v>
+      </c>
+      <c r="G15" s="6">
+        <v>3</v>
+      </c>
       <c r="H15" s="6">
         <v>3</v>
       </c>
@@ -939,15 +975,21 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="E16" s="6">
+        <v>3</v>
+      </c>
+      <c r="F16" s="6">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6">
+        <v>3</v>
+      </c>
       <c r="H16" s="6">
         <v>3</v>
       </c>
@@ -961,9 +1003,15 @@
       <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6">
+        <v>3</v>
+      </c>
       <c r="H17" s="6">
         <v>1</v>
       </c>
@@ -971,13 +1019,15 @@
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>3</v>
+      </c>
       <c r="F18" s="6">
         <v>3</v>
       </c>
@@ -991,17 +1041,21 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
       <c r="F19" s="6">
         <v>3</v>
       </c>
-      <c r="G19" s="6"/>
+      <c r="G19" s="6">
+        <v>3</v>
+      </c>
       <c r="H19" s="6">
         <v>3</v>
       </c>
@@ -1009,13 +1063,15 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>2</v>
+      </c>
       <c r="F20" s="6">
         <v>3</v>
       </c>
@@ -1029,17 +1085,21 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6">
         <v>1</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>3</v>
+      </c>
       <c r="F21" s="6">
         <v>3</v>
       </c>
-      <c r="G21" s="6"/>
+      <c r="G21" s="6">
+        <v>3</v>
+      </c>
       <c r="H21" s="6">
         <v>0</v>
       </c>
@@ -1047,13 +1107,19 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="6">
+        <v>3</v>
+      </c>
+      <c r="F22" s="6">
+        <v>3</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2</v>
+      </c>
       <c r="H22" s="6">
         <v>2</v>
       </c>
@@ -1067,7 +1133,9 @@
         <v>1</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>2</v>
+      </c>
       <c r="F23" s="6">
         <v>3</v>
       </c>
@@ -1081,17 +1149,21 @@
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
         <v>1</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6">
+        <v>3</v>
+      </c>
       <c r="F24" s="6">
         <v>3</v>
       </c>
-      <c r="G24" s="6"/>
+      <c r="G24" s="6">
+        <v>2</v>
+      </c>
       <c r="H24" s="6">
         <v>0</v>
       </c>
@@ -1105,11 +1177,15 @@
       <c r="D25" s="6">
         <v>1</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6">
+        <v>3</v>
+      </c>
       <c r="F25" s="6">
         <v>3</v>
       </c>
-      <c r="G25" s="6"/>
+      <c r="G25" s="6">
+        <v>3</v>
+      </c>
       <c r="H25" s="6">
         <v>1</v>
       </c>
@@ -1117,7 +1193,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6">
@@ -1125,7 +1201,9 @@
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="G26" s="6">
+        <v>3</v>
+      </c>
       <c r="H26" s="6">
         <v>3</v>
       </c>
@@ -1133,7 +1211,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6">
@@ -1155,17 +1233,21 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6">
+        <v>2</v>
+      </c>
       <c r="F28" s="6">
         <v>2</v>
       </c>
-      <c r="G28" s="6"/>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
       <c r="H28" s="6">
         <v>1</v>
       </c>
@@ -1173,17 +1255,21 @@
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6">
         <v>1</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6">
+        <v>2</v>
+      </c>
       <c r="F29" s="6">
         <v>2</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" s="6">
+        <v>2</v>
+      </c>
       <c r="H29" s="6">
         <v>1</v>
       </c>
@@ -1191,13 +1277,15 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>1</v>
       </c>
-      <c r="E30" s="6"/>
+      <c r="E30" s="6">
+        <v>3</v>
+      </c>
       <c r="F30" s="6">
         <v>2</v>
       </c>
@@ -1211,13 +1299,15 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6">
         <v>1</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6">
+        <v>3</v>
+      </c>
       <c r="F31" s="6">
         <v>2</v>
       </c>
@@ -1264,17 +1354,21 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6">
         <v>1</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6">
+        <v>1</v>
+      </c>
       <c r="F34" s="6">
         <v>3</v>
       </c>
-      <c r="G34" s="6"/>
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
       <c r="H34" s="6">
         <v>1</v>
       </c>
@@ -1282,17 +1376,21 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6">
         <v>1</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
       <c r="F35" s="6">
         <v>3</v>
       </c>
-      <c r="G35" s="6"/>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
       <c r="H35" s="6">
         <v>2</v>
       </c>
@@ -1308,10 +1406,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6">
@@ -1333,7 +1431,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6">
@@ -1355,13 +1453,15 @@
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6">
         <v>1</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="6">
+        <v>2</v>
+      </c>
       <c r="F39" s="6">
         <v>3</v>
       </c>
@@ -1386,15 +1486,21 @@
         <v>25</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="6">
         <v>1</v>
       </c>
       <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="E41" s="6">
+        <v>1</v>
+      </c>
+      <c r="F41" s="6">
+        <v>3</v>
+      </c>
+      <c r="G41" s="6">
+        <v>3</v>
+      </c>
       <c r="H41" s="6">
         <v>3</v>
       </c>
@@ -1402,15 +1508,21 @@
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" s="6">
         <v>1</v>
       </c>
       <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="E42" s="6">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6">
+        <v>3</v>
+      </c>
+      <c r="G42" s="6">
+        <v>3</v>
+      </c>
       <c r="H42" s="6">
         <v>3</v>
       </c>
@@ -1418,15 +1530,21 @@
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="E43" s="6">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6">
+        <v>3</v>
+      </c>
+      <c r="G43" s="6">
+        <v>1</v>
+      </c>
       <c r="H43" s="6">
         <v>1</v>
       </c>
@@ -1445,15 +1563,21 @@
         <v>23</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6">
         <v>1</v>
       </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="E45" s="6">
+        <v>2</v>
+      </c>
+      <c r="F45" s="6">
+        <v>2</v>
+      </c>
+      <c r="G45" s="6">
+        <v>2</v>
+      </c>
       <c r="H45" s="6">
         <v>3</v>
       </c>
@@ -1461,7 +1585,7 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="6">
         <v>1</v>
@@ -1544,7 +1668,9 @@
       <c r="D50" s="6">
         <v>1</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="6">
+        <v>2</v>
+      </c>
       <c r="F50" s="6">
         <v>3</v>
       </c>
@@ -1558,15 +1684,21 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6">
         <v>1</v>
       </c>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="E51" s="6">
+        <v>2</v>
+      </c>
+      <c r="F51" s="6">
+        <v>3</v>
+      </c>
+      <c r="G51" s="6">
+        <v>3</v>
+      </c>
       <c r="H51" s="6">
         <v>1</v>
       </c>
@@ -1574,15 +1706,21 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C52" s="6">
         <v>1</v>
       </c>
       <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="E52" s="6">
+        <v>3</v>
+      </c>
+      <c r="F52" s="6">
+        <v>3</v>
+      </c>
+      <c r="G52" s="6">
+        <v>3</v>
+      </c>
       <c r="H52" s="6">
         <v>1</v>
       </c>
@@ -1623,15 +1761,15 @@
       </c>
       <c r="E55" s="1">
         <f>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[ZABBIX])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[ZABBIX]))</f>
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="F55" s="1">
         <f>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[NAGIOS XI])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[NAGIOS XI]))</f>
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="G55" s="1">
         <f>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[CENTREON])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[CENTREON]))</f>
-        <v>97</v>
+        <v>203</v>
       </c>
       <c r="H55" s="1">
         <f>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[IPMONITOR])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[IPMONITOR]))</f>

</xml_diff>

<commit_message>
"Mise à jour de l'étude comparative. En attente d'une dernière correction"
</commit_message>
<xml_diff>
--- a/etude-comparative/comparatif.xlsx
+++ b/etude-comparative/comparatif.xlsx
@@ -245,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,11 +269,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -305,12 +329,6 @@
       <font>
         <b/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -353,19 +371,19 @@
   <autoFilter ref="A1:H54"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Catégorie" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Caractéristique" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Caractéristique" dataDxfId="18" totalsRowDxfId="6"/>
     <tableColumn id="3" name="pré-requis" dataDxfId="17"/>
     <tableColumn id="4" name="optionnel" dataDxfId="16"/>
-    <tableColumn id="5" name="ZABBIX" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="3">
+    <tableColumn id="5" name="ZABBIX" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="5">
       <totalsRowFormula>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[ZABBIX])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[ZABBIX]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="NAGIOS XI" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="2">
+    <tableColumn id="6" name="NAGIOS XI" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="4">
       <totalsRowFormula>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[NAGIOS XI])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[NAGIOS XI]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="CENTREON" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="1">
+    <tableColumn id="7" name="CENTREON" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="3">
       <totalsRowFormula>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[CENTREON])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[CENTREON]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="IPMONITOR" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="0">
+    <tableColumn id="8" name="IPMONITOR" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="2">
       <totalsRowFormula>SUM(SUMPRODUCT(Tableau1[pré-requis],Tableau1[IPMONITOR])*3,SUMPRODUCT(Tableau1[optionnel],Tableau1[IPMONITOR]))</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -374,14 +392,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B59:F66" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B59:F66" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
   <autoFilter ref="B59:F66"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Catégorie" dataDxfId="9"/>
-    <tableColumn id="2" name="ZABBIX" dataDxfId="8"/>
-    <tableColumn id="3" name="NAGIOS XI" dataDxfId="7"/>
-    <tableColumn id="4" name="CENTREON" dataDxfId="6"/>
-    <tableColumn id="5" name="IPMONITOR" dataDxfId="5"/>
+    <tableColumn id="1" name="Catégorie" dataDxfId="11"/>
+    <tableColumn id="2" name="ZABBIX" dataDxfId="10"/>
+    <tableColumn id="3" name="NAGIOS XI" dataDxfId="9"/>
+    <tableColumn id="4" name="CENTREON" dataDxfId="8"/>
+    <tableColumn id="5" name="IPMONITOR" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -676,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F59" sqref="C59:F59"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F66" sqref="B59:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,20 +1841,21 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="58" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D59" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
-        <v>2</v>
-      </c>
-      <c r="F59" s="1" t="s">
+      <c r="D59" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G59"/>
@@ -1977,13 +1996,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E5:H54 E4:G4 E2:H3">
-    <cfRule type="iconSet" priority="58">
+    <cfRule type="iconSet" priority="59">
       <iconSet iconSet="4TrafficLights" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
       </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:F66">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1996,7 +2027,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="31" id="{ECF5901B-A7D2-450A-B24B-BB8389D6E5E3}">
+          <x14:cfRule type="iconSet" priority="32" id="{ECF5901B-A7D2-450A-B24B-BB8389D6E5E3}">
             <x14:iconSet iconSet="3Stars" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -2012,7 +2043,7 @@
           <xm:sqref>C2:D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="56" id="{DF82DF9A-923A-4424-9DE1-4294FD97DF01}">
+          <x14:cfRule type="iconSet" priority="57" id="{DF82DF9A-923A-4424-9DE1-4294FD97DF01}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>

</xml_diff>